<commit_message>
Changed Brand to Kato
</commit_message>
<xml_diff>
--- a/amazon_co-ecommerce_sample(7).xlsx
+++ b/amazon_co-ecommerce_sample(7).xlsx
@@ -6402,8 +6402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F7098"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -6661,7 +6661,7 @@
         <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="D13">
         <v>273.60000000000002</v>
@@ -6681,7 +6681,7 @@
         <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="D14">
         <v>9.6</v>

</xml_diff>